<commit_message>
added control for end_sample in local vintages
</commit_message>
<xml_diff>
--- a/models/US_no_core_rt/data/US_local.xlsx
+++ b/models/US_no_core_rt/data/US_local.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Documents/Shared/Nowcasting stargate/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fpellegrino/Desktop/inflation_mixed_freq/models/US_no_core_rt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6FDA98D-3596-1543-988E-1073A137B6FE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33A027A5-DB65-3C42-9A24-302CE5359E7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="20920" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16880" yWindow="460" windowWidth="20920" windowHeight="16240" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="monthly" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="909" uniqueCount="647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="648">
   <si>
     <t>ASACX1@HAVER</t>
   </si>
@@ -1982,6 +1982,9 @@
   </si>
   <si>
     <t>Jun-2020</t>
+  </si>
+  <si>
+    <t>Variables</t>
   </si>
 </sst>
 </file>
@@ -2088,7 +2091,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2122,6 +2125,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="8" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Explanatory Text 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
@@ -2465,7 +2469,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C444"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -15739,7 +15743,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:AJO4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
@@ -15751,6 +15757,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:951" s="5" customFormat="1" ht="16" customHeight="1">
+      <c r="A1" s="21" t="s">
+        <v>647</v>
+      </c>
       <c r="B1" s="12">
         <v>38260</v>
       </c>

</xml_diff>